<commit_message>
typo in replicate names
</commit_message>
<xml_diff>
--- a/File Naming.xlsx
+++ b/File Naming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\curly\Desktop\Apple Genotyping\Experiments\Renaming Sample Labels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4164DE-3DFB-4A5E-B9B7-62409AED889C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDB1EE2-BEC4-4A50-9694-8E0CA74029BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{3491D669-C83C-4979-B15B-06B44BE9C919}"/>
   </bookViews>
@@ -4667,168 +4667,45 @@
     <t>BBQ1654_P17_(Axiom_JKI50kMd)_P17.CEL</t>
   </si>
   <si>
-    <t>Merton Russet.CEL</t>
-  </si>
-  <si>
     <t>Oriole.CEL</t>
   </si>
   <si>
     <t>Gewerzluikenapfel.CEL</t>
   </si>
   <si>
-    <t>Hajkovo Muskatove.CEL</t>
-  </si>
-  <si>
     <t>Abas.CEL</t>
   </si>
   <si>
-    <t>Golden Russet.CEL</t>
-  </si>
-  <si>
     <t>Rosemund.CEL</t>
   </si>
   <si>
     <t>Winston.CEL</t>
   </si>
   <si>
-    <t>Glockenapfel eckter.CEL</t>
-  </si>
-  <si>
-    <t>Kingston Black.CEL</t>
-  </si>
-  <si>
-    <t>Cambridge Pippin.CEL</t>
-  </si>
-  <si>
-    <t>Northern Spy.CEL</t>
-  </si>
-  <si>
-    <t>Springrove Codlin.CEL</t>
-  </si>
-  <si>
-    <t>French Crab.CEL</t>
-  </si>
-  <si>
-    <t>Besterfielder Renette.CEL</t>
-  </si>
-  <si>
-    <t>Uster Gloria.CEL</t>
-  </si>
-  <si>
-    <t>Altainder Plannkuchenapfel.CEL</t>
-  </si>
-  <si>
     <t>Lobo.CEL</t>
   </si>
   <si>
-    <t>Stayman's Winesap.CEL</t>
-  </si>
-  <si>
-    <t>Geeveston Fanny.CEL</t>
-  </si>
-  <si>
-    <t>Green Square.CEL</t>
-  </si>
-  <si>
-    <t>Fleuritard Rouge.CEL</t>
-  </si>
-  <si>
-    <t>Malus kaido.CEL</t>
-  </si>
-  <si>
     <t>Dietrecht.CEL</t>
   </si>
   <si>
     <t>Spivey.CEL</t>
   </si>
   <si>
-    <t>Nancy's Favourite.CEL</t>
-  </si>
-  <si>
-    <t>Shorland Queen.CEL</t>
-  </si>
-  <si>
-    <t>Wilmont Russet.CEL</t>
-  </si>
-  <si>
-    <t>Warner's King.CEL</t>
-  </si>
-  <si>
-    <t>Grimes Golden.CEL</t>
-  </si>
-  <si>
     <t>Hetlina.CEL</t>
   </si>
   <si>
     <t>Sunglo.CEL</t>
   </si>
   <si>
-    <t>The Doctor.CEL</t>
-  </si>
-  <si>
     <t>Catshead.CEL</t>
   </si>
   <si>
     <t>Astrachan.CEL</t>
   </si>
   <si>
-    <t>Egremont Russet.CEL</t>
-  </si>
-  <si>
-    <t>Tydeman’s Late Orange.CEL</t>
-  </si>
-  <si>
-    <t>Ellison's Orange.CEL</t>
-  </si>
-  <si>
-    <t>Malus boccata gracilis.CEL</t>
-  </si>
-  <si>
-    <t>Golden Noble.CEL</t>
-  </si>
-  <si>
-    <t>Lord Lambourne .CEL</t>
-  </si>
-  <si>
-    <t>Kentish Fillbasket.CEL</t>
-  </si>
-  <si>
     <t>Melrose.CEL</t>
   </si>
   <si>
-    <t>Maggie Grieve.CEL</t>
-  </si>
-  <si>
-    <t>Calville Blanc d'Hiver.CEL</t>
-  </si>
-  <si>
-    <t>Flower of Kent.CEL</t>
-  </si>
-  <si>
-    <t>William Crump.CEL</t>
-  </si>
-  <si>
-    <t>Belle de Boskoop.CEL</t>
-  </si>
-  <si>
-    <t>Peasgood Nonsuch.CEL</t>
-  </si>
-  <si>
-    <t>Malus floribunda.CEL</t>
-  </si>
-  <si>
-    <t>Bramley's Seedling.CEL</t>
-  </si>
-  <si>
-    <t>Sintax Alkmene.CEL</t>
-  </si>
-  <si>
-    <t>Lady Hamilton Sth..CEL</t>
-  </si>
-  <si>
-    <t>Mother in Law.CEL</t>
-  </si>
-  <si>
     <t>Democrat.CEL</t>
   </si>
   <si>
@@ -4838,48 +4715,18 @@
     <t>Rymer.CEL</t>
   </si>
   <si>
-    <t>Camoesa De Llobregat.CEL</t>
-  </si>
-  <si>
-    <t>Ribston Pippin.CEL</t>
-  </si>
-  <si>
-    <t>Tydeman's Early Worcester.CEL</t>
-  </si>
-  <si>
-    <t>Rhode Island Greening.CEL</t>
-  </si>
-  <si>
     <t>Brighton.CEL</t>
   </si>
   <si>
     <t>Cloden.CEL</t>
   </si>
   <si>
-    <t>Scarlett Pearmain.CEL</t>
-  </si>
-  <si>
     <t>Paneske.CEL</t>
   </si>
   <si>
-    <t>William Anderson.CEL</t>
-  </si>
-  <si>
     <t>Sciros.CEL</t>
   </si>
   <si>
-    <t>Alma Pippin.CEL</t>
-  </si>
-  <si>
-    <t>Gloria Mundy.CEL</t>
-  </si>
-  <si>
-    <t>Jupp's Russet.CEL</t>
-  </si>
-  <si>
-    <t>Gold Strike.CEL</t>
-  </si>
-  <si>
     <t>Discovery.CEL</t>
   </si>
   <si>
@@ -4892,33 +4739,12 @@
     <t>Fairbelle.CEL</t>
   </si>
   <si>
-    <t>Winter Banana.CEL</t>
-  </si>
-  <si>
-    <t>Brabantse Bellefleur.CEL</t>
-  </si>
-  <si>
-    <t>Twenty Ounce.CEL</t>
-  </si>
-  <si>
     <t>Ballarat.CEL</t>
   </si>
   <si>
-    <t>Beautiful Arcade.CEL</t>
-  </si>
-  <si>
     <t>Hawthornden.CEL</t>
   </si>
   <si>
-    <t>Blenhiem Orange.CEL</t>
-  </si>
-  <si>
-    <t>Monty's Surprise.CEL</t>
-  </si>
-  <si>
-    <t>Kidd's Orange.CEL</t>
-  </si>
-  <si>
     <t>Sunset.CEL</t>
   </si>
   <si>
@@ -4928,60 +4754,18 @@
     <t>Splendour.CEL</t>
   </si>
   <si>
-    <t>Gene Pitney.CEL</t>
-  </si>
-  <si>
-    <t>Sheppard Perfection.CEL</t>
-  </si>
-  <si>
-    <t>Rome Beauty.CEL</t>
-  </si>
-  <si>
-    <t>Scarlet Nonpareil.CEL</t>
-  </si>
-  <si>
     <t>Grenadier.CEL</t>
   </si>
   <si>
-    <t>Tower of Glamis.CEL</t>
-  </si>
-  <si>
-    <t>Red Astrachan.CEL</t>
-  </si>
-  <si>
-    <t>Rall's Janet.CEL</t>
-  </si>
-  <si>
-    <t>Sir Prize.CEL</t>
-  </si>
-  <si>
-    <t>Yellow Bellflower.CEL</t>
-  </si>
-  <si>
-    <t>Roja de Valle Benejama.CEL</t>
-  </si>
-  <si>
     <t>Shamrock.CEL</t>
   </si>
   <si>
-    <t>Malus aldenhanmi.CEL</t>
-  </si>
-  <si>
     <t>Washington.CEL</t>
   </si>
   <si>
-    <t>Granny Smith.CEL</t>
-  </si>
-  <si>
-    <t>Queen Mary.CEL</t>
-  </si>
-  <si>
     <t>Nonpareil.CEL</t>
   </si>
   <si>
-    <t>Nonetit Bastard.CEL</t>
-  </si>
-  <si>
     <t>Springdale.CEL</t>
   </si>
   <si>
@@ -4991,42 +4775,9 @@
     <t>Richared.CEL</t>
   </si>
   <si>
-    <t>Beauty of Kent.CEL</t>
-  </si>
-  <si>
     <t>Close.CEL</t>
   </si>
   <si>
-    <t>Woolbrook Pippin.CEL</t>
-  </si>
-  <si>
-    <t>Rosa du Perche.CEL</t>
-  </si>
-  <si>
-    <t>Monroes Favourite.CEL</t>
-  </si>
-  <si>
-    <t>Cornish Aromatic.CEL</t>
-  </si>
-  <si>
-    <t>Albany Beauty.CEL</t>
-  </si>
-  <si>
-    <t>C'Huero Ru Bien.CEL</t>
-  </si>
-  <si>
-    <t>Reinette du Canada.CEL</t>
-  </si>
-  <si>
-    <t>Black Twig.CEL</t>
-  </si>
-  <si>
-    <t>Belle Bonne.CEL</t>
-  </si>
-  <si>
-    <t>Golden Pippin.CEL</t>
-  </si>
-  <si>
     <t>Eklinville.CEL</t>
   </si>
   <si>
@@ -5036,129 +4787,51 @@
     <t>Cortland.CEL</t>
   </si>
   <si>
-    <t>Laxton's Superb.CEL</t>
-  </si>
-  <si>
-    <t>Scarlett Pimpernel.CEL</t>
-  </si>
-  <si>
-    <t>Jack Humm.CEL</t>
-  </si>
-  <si>
-    <t>Karmajin de Sonnaville.CEL</t>
-  </si>
-  <si>
-    <t>Lord Derby.CEL</t>
-  </si>
-  <si>
-    <t>Newtown Pippin.CEL</t>
-  </si>
-  <si>
-    <t>Bordes (cider).CEL</t>
-  </si>
-  <si>
     <t>Alice.CEL</t>
   </si>
   <si>
     <t>Priscilla.CEL</t>
   </si>
   <si>
-    <t>Bisquet (cider).CEL</t>
-  </si>
-  <si>
-    <t>Geheimrat Breuhahn.CEL</t>
-  </si>
-  <si>
-    <t>George Neale.CEL</t>
-  </si>
-  <si>
     <t>Lodi.CEL</t>
   </si>
   <si>
-    <t>Allen's Everlasting.CEL</t>
-  </si>
-  <si>
     <t>Fuji.CEL</t>
   </si>
   <si>
-    <t>Lord Wolseley .CEL</t>
-  </si>
-  <si>
     <t>Raritan.CEL</t>
   </si>
   <si>
-    <t>Esopus Spitzenburg.CEL</t>
-  </si>
-  <si>
     <t>Freyberg.CEL</t>
   </si>
   <si>
-    <t>Sweet Alford.CEL</t>
-  </si>
-  <si>
-    <t>Red Baron.CEL</t>
-  </si>
-  <si>
-    <t>Red Dougherty.CEL</t>
-  </si>
-  <si>
-    <t>Malus micromalus.CEL</t>
-  </si>
-  <si>
     <t>Salome.CEL</t>
   </si>
   <si>
     <t>Bonza.CEL</t>
   </si>
   <si>
-    <t>Black Prince.CEL</t>
-  </si>
-  <si>
     <t>Charlotte.CEL</t>
   </si>
   <si>
-    <t>Irish Peach.CEL</t>
-  </si>
-  <si>
     <t>Jonathan.CEL</t>
   </si>
   <si>
     <t>Chieftan.CEL</t>
   </si>
   <si>
-    <t>Worcester Pearmain.CEL</t>
-  </si>
-  <si>
     <t>Bismark.CEL</t>
   </si>
   <si>
     <t>Spartan.CEL</t>
   </si>
   <si>
-    <t>Bozena Nemcova.CEL</t>
-  </si>
-  <si>
-    <t>Golden Harvest.CEL</t>
-  </si>
-  <si>
-    <t>Saint Magdalen.CEL</t>
-  </si>
-  <si>
     <t>Mother.CEL</t>
   </si>
   <si>
     <t>Charden.CEL</t>
   </si>
   <si>
-    <t>M. robusta 5.CEL</t>
-  </si>
-  <si>
-    <t>Stemphered Pippin.CEL</t>
-  </si>
-  <si>
-    <t>Royal Gala.CEL</t>
-  </si>
-  <si>
     <t>Alkmene.CEL</t>
   </si>
   <si>
@@ -5174,9 +4847,6 @@
     <t>PremA129.CEL</t>
   </si>
   <si>
-    <t>M. baccata jackii.CEL</t>
-  </si>
-  <si>
     <t>A209R08T022.CEL</t>
   </si>
   <si>
@@ -5198,6 +4868,339 @@
     <t>PremA153.CEL</t>
   </si>
   <si>
+    <t>Woolbrook_Pippin.CEL</t>
+  </si>
+  <si>
+    <t>Worcester_Pearmain.CEL</t>
+  </si>
+  <si>
+    <t>Yellow_Bellflower.CEL</t>
+  </si>
+  <si>
+    <t>Albany_Beauty.CEL</t>
+  </si>
+  <si>
+    <t>Allen's_Everlasting.CEL</t>
+  </si>
+  <si>
+    <t>Alma_Pippin.CEL</t>
+  </si>
+  <si>
+    <t>Altainder_Plannkuchenapfel.CEL</t>
+  </si>
+  <si>
+    <t>Beautiful_Arcade.CEL</t>
+  </si>
+  <si>
+    <t>Beauty_of_Kent.CEL</t>
+  </si>
+  <si>
+    <t>Belle_Bonne.CEL</t>
+  </si>
+  <si>
+    <t>Belle_de_Boskoop.CEL</t>
+  </si>
+  <si>
+    <t>Besterfielder_Renette.CEL</t>
+  </si>
+  <si>
+    <t>Bisquet_(cider).CEL</t>
+  </si>
+  <si>
+    <t>Black_Prince.CEL</t>
+  </si>
+  <si>
+    <t>Black_Twig.CEL</t>
+  </si>
+  <si>
+    <t>Blenhiem_Orange.CEL</t>
+  </si>
+  <si>
+    <t>Bordes_(cider).CEL</t>
+  </si>
+  <si>
+    <t>Bozena_Nemcova.CEL</t>
+  </si>
+  <si>
+    <t>Brabantse_Bellefleur.CEL</t>
+  </si>
+  <si>
+    <t>Bramley's_Seedling.CEL</t>
+  </si>
+  <si>
+    <t>Calville_Blanc_d'Hiver.CEL</t>
+  </si>
+  <si>
+    <t>Cambridge_Pippin.CEL</t>
+  </si>
+  <si>
+    <t>Camoesa_De_Llobregat.CEL</t>
+  </si>
+  <si>
+    <t>C'Huero_Ru_Bien.CEL</t>
+  </si>
+  <si>
+    <t>Cornish_Aromatic.CEL</t>
+  </si>
+  <si>
+    <t>Egremont_Russet.CEL</t>
+  </si>
+  <si>
+    <t>Ellison's_Orange.CEL</t>
+  </si>
+  <si>
+    <t>Esopus_Spitzenburg.CEL</t>
+  </si>
+  <si>
+    <t>Fleuritard_Rouge.CEL</t>
+  </si>
+  <si>
+    <t>Flower_of_Kent.CEL</t>
+  </si>
+  <si>
+    <t>French_Crab.CEL</t>
+  </si>
+  <si>
+    <t>Geeveston_Fanny.CEL</t>
+  </si>
+  <si>
+    <t>Geheimrat_Breuhahn.CEL</t>
+  </si>
+  <si>
+    <t>Gene_Pitney.CEL</t>
+  </si>
+  <si>
+    <t>George_Neale.CEL</t>
+  </si>
+  <si>
+    <t>Glockenapfel_eckter.CEL</t>
+  </si>
+  <si>
+    <t>Gloria_Mundy.CEL</t>
+  </si>
+  <si>
+    <t>Gold_Strike.CEL</t>
+  </si>
+  <si>
+    <t>Golden_Harvest.CEL</t>
+  </si>
+  <si>
+    <t>Golden_Noble.CEL</t>
+  </si>
+  <si>
+    <t>Golden_Pippin.CEL</t>
+  </si>
+  <si>
+    <t>Golden_Russet.CEL</t>
+  </si>
+  <si>
+    <t>Granny_Smith.CEL</t>
+  </si>
+  <si>
+    <t>Green_Square.CEL</t>
+  </si>
+  <si>
+    <t>Grimes_Golden.CEL</t>
+  </si>
+  <si>
+    <t>Hajkovo_Muskatove.CEL</t>
+  </si>
+  <si>
+    <t>Irish_Peach.CEL</t>
+  </si>
+  <si>
+    <t>Jack_Humm.CEL</t>
+  </si>
+  <si>
+    <t>Jupp's_Russet.CEL</t>
+  </si>
+  <si>
+    <t>Karmajin_de_Sonnaville.CEL</t>
+  </si>
+  <si>
+    <t>Kentish_Fillbasket.CEL</t>
+  </si>
+  <si>
+    <t>Kidd's_Orange.CEL</t>
+  </si>
+  <si>
+    <t>Kingston_Black.CEL</t>
+  </si>
+  <si>
+    <t>Lady_Hamilton_Sth..CEL</t>
+  </si>
+  <si>
+    <t>Laxton's_Superb.CEL</t>
+  </si>
+  <si>
+    <t>Lord_Derby.CEL</t>
+  </si>
+  <si>
+    <t>Lord_Lambourne_.CEL</t>
+  </si>
+  <si>
+    <t>Lord_Wolseley_.CEL</t>
+  </si>
+  <si>
+    <t>M._baccata_jackii.CEL</t>
+  </si>
+  <si>
+    <t>M._robusta_5.CEL</t>
+  </si>
+  <si>
+    <t>Maggie_Grieve.CEL</t>
+  </si>
+  <si>
+    <t>Malus_aldenhanmi.CEL</t>
+  </si>
+  <si>
+    <t>Malus_boccata_gracilis.CEL</t>
+  </si>
+  <si>
+    <t>Malus_floribunda.CEL</t>
+  </si>
+  <si>
+    <t>Malus_kaido.CEL</t>
+  </si>
+  <si>
+    <t>Malus_micromalus.CEL</t>
+  </si>
+  <si>
+    <t>Malus_pumila_Niedzwetzkyana.CEL</t>
+  </si>
+  <si>
+    <t>Merton_Russet.CEL</t>
+  </si>
+  <si>
+    <t>Monroes_Favourite.CEL</t>
+  </si>
+  <si>
+    <t>Monty's_Surprise.CEL</t>
+  </si>
+  <si>
+    <t>Mother_in_Law.CEL</t>
+  </si>
+  <si>
+    <t>Nancy's_Favourite.CEL</t>
+  </si>
+  <si>
+    <t>Newtown_Pippin.CEL</t>
+  </si>
+  <si>
+    <t>Nonetit_Bastard.CEL</t>
+  </si>
+  <si>
+    <t>Northern_Spy.CEL</t>
+  </si>
+  <si>
+    <t>Peasgood_Nonsuch.CEL</t>
+  </si>
+  <si>
+    <t>Queen_Mary.CEL</t>
+  </si>
+  <si>
+    <t>Rall's_Janet.CEL</t>
+  </si>
+  <si>
+    <t>Red_Astrachan.CEL</t>
+  </si>
+  <si>
+    <t>Red_Baron.CEL</t>
+  </si>
+  <si>
+    <t>Red_Dougherty.CEL</t>
+  </si>
+  <si>
+    <t>Reinette_du_Canada.CEL</t>
+  </si>
+  <si>
+    <t>Rhode_Island_Greening.CEL</t>
+  </si>
+  <si>
+    <t>Ribston_Pippin.CEL</t>
+  </si>
+  <si>
+    <t>Roja_de_Valle_Benejama.CEL</t>
+  </si>
+  <si>
+    <t>Rome_Beauty.CEL</t>
+  </si>
+  <si>
+    <t>Rosa_du_Perche.CEL</t>
+  </si>
+  <si>
+    <t>Royal_Gala.CEL</t>
+  </si>
+  <si>
+    <t>Saint_Magdalen.CEL</t>
+  </si>
+  <si>
+    <t>Scarlet_Nonpareil.CEL</t>
+  </si>
+  <si>
+    <t>Scarlett_Pearmain.CEL</t>
+  </si>
+  <si>
+    <t>Scarlett_Pimpernel.CEL</t>
+  </si>
+  <si>
+    <t>Sheppard_Perfection.CEL</t>
+  </si>
+  <si>
+    <t>Shorland_Queen.CEL</t>
+  </si>
+  <si>
+    <t>Sintax_Alkmene.CEL</t>
+  </si>
+  <si>
+    <t>Sir_Prize.CEL</t>
+  </si>
+  <si>
+    <t>Springrove_Codlin.CEL</t>
+  </si>
+  <si>
+    <t>Stayman's_Winesap.CEL</t>
+  </si>
+  <si>
+    <t>Stemphered_Pippin.CEL</t>
+  </si>
+  <si>
+    <t>Sweet_Alford.CEL</t>
+  </si>
+  <si>
+    <t>The_Doctor.CEL</t>
+  </si>
+  <si>
+    <t>Tower_of_Glamis.CEL</t>
+  </si>
+  <si>
+    <t>Twenty_Ounce.CEL</t>
+  </si>
+  <si>
+    <t>Tydeman’s_Late_Orange.CEL</t>
+  </si>
+  <si>
+    <t>Tydeman's_Early_Worcester.CEL</t>
+  </si>
+  <si>
+    <t>Uster_Gloria.CEL</t>
+  </si>
+  <si>
+    <t>Warner's_King.CEL</t>
+  </si>
+  <si>
+    <t>William_Anderson.CEL</t>
+  </si>
+  <si>
+    <t>William_Crump.CEL</t>
+  </si>
+  <si>
+    <t>Wilmont_Russet.CEL</t>
+  </si>
+  <si>
+    <t>Winter_Banana.CEL</t>
+  </si>
+  <si>
     <t>A101R08T016_rep.CEL</t>
   </si>
   <si>
@@ -5216,34 +5219,31 @@
     <t>A569R10T144_rep.CEL</t>
   </si>
   <si>
-    <t>M. baccata jackii_rep.CEL</t>
-  </si>
-  <si>
-    <t>M. robusta 5_rep.CEL</t>
-  </si>
-  <si>
-    <t>M. robusta 5_rep2.CEL</t>
+    <t>M._baccata_jackii_rep.CEL</t>
+  </si>
+  <si>
+    <t>Tydeman's_Late_Orange_rep.CEL</t>
+  </si>
+  <si>
+    <t>Sciros_rep.CEL</t>
+  </si>
+  <si>
+    <t>PremA153_rep.CEL</t>
+  </si>
+  <si>
+    <t>PremA129_rep.CEL</t>
   </si>
   <si>
     <t>M9_rep.CEL</t>
   </si>
   <si>
-    <t>Malus pumila Niedzwetzkyana.CEL</t>
-  </si>
-  <si>
-    <t>PremA129_rep.CEL</t>
-  </si>
-  <si>
-    <t>PremA153_rep.CEL</t>
-  </si>
-  <si>
-    <t>Sciros_rep.CEL</t>
+    <t>M._robusta_5_rep.CEL</t>
   </si>
   <si>
     <t>Sciros_rep2.CEL</t>
   </si>
   <si>
-    <t>Tydeman's Late Orange_rep.CEL</t>
+    <t>M._robusta_5_rep2.CEL</t>
   </si>
 </sst>
 </file>
@@ -5669,9 +5669,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F337"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H192" sqref="H192"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5721,7 +5721,7 @@
         <v>1524</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1714</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -5741,7 +5741,7 @@
         <v>1531</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>1720</v>
+        <v>1721</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -5761,7 +5761,7 @@
         <v>1523</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>1713</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -5781,7 +5781,7 @@
         <v>1535</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>1721</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -5801,7 +5801,7 @@
         <v>1532</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>1718</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -5821,7 +5821,7 @@
         <v>1541</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>1722</v>
+        <v>1723</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -5841,7 +5841,7 @@
         <v>1519</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>1710</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -5861,7 +5861,7 @@
         <v>1538</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>1723</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -5881,7 +5881,7 @@
         <v>1529</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>1717</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -5901,7 +5901,7 @@
         <v>1536</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>1724</v>
+        <v>1725</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -5921,7 +5921,7 @@
         <v>1526</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>1715</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -5941,7 +5941,7 @@
         <v>1534</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>1725</v>
+        <v>1726</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -5961,7 +5961,7 @@
         <v>1350</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>1547</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -5981,7 +5981,7 @@
         <v>1420</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>1616</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -6001,7 +6001,7 @@
         <v>1514</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>1709</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -6021,7 +6021,7 @@
         <v>1462</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>1657</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -6041,7 +6041,7 @@
         <v>1478</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>1673</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -6061,7 +6061,7 @@
         <v>1512</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>1707</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -6081,7 +6081,7 @@
         <v>1484</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>1679</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -6101,7 +6101,7 @@
         <v>1414</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>1610</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -6121,7 +6121,7 @@
         <v>1362</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>1559</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -6141,7 +6141,7 @@
         <v>1380</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>1577</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -6161,7 +6161,7 @@
         <v>1425</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>1621</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -6181,7 +6181,7 @@
         <v>1426</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>1622</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -6201,7 +6201,7 @@
         <v>1456</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>1651</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -6221,7 +6221,7 @@
         <v>1466</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>1661</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
@@ -6241,7 +6241,7 @@
         <v>1394</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>1590</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -6261,7 +6261,7 @@
         <v>1360</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>1557</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -6281,7 +6281,7 @@
         <v>1502</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>1697</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -6301,7 +6301,7 @@
         <v>1480</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>1675</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -6321,7 +6321,7 @@
         <v>1496</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>1691</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -6341,7 +6341,7 @@
         <v>1465</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>1660</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -6361,7 +6361,7 @@
         <v>1419</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>1615</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -6381,7 +6381,7 @@
         <v>1428</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>1624</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -6401,7 +6401,7 @@
         <v>1495</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>1690</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -6421,7 +6421,7 @@
         <v>1477</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>1672</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
@@ -6441,7 +6441,7 @@
         <v>1504</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>1699</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -6461,7 +6461,7 @@
         <v>1423</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>1619</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -6481,7 +6481,7 @@
         <v>1397</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>1593</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -6501,7 +6501,7 @@
         <v>1408</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>1604</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -6521,7 +6521,7 @@
         <v>1391</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>1587</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -6541,7 +6541,7 @@
         <v>1356</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>1553</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -6561,7 +6561,7 @@
         <v>1404</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>1600</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -6581,7 +6581,7 @@
         <v>1379</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>1576</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -6601,7 +6601,7 @@
         <v>1508</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>1703</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
@@ -6621,7 +6621,7 @@
         <v>1497</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>1692</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -6641,7 +6641,7 @@
         <v>1500</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>1695</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -6661,7 +6661,7 @@
         <v>1463</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>1658</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -6681,7 +6681,7 @@
         <v>1409</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>1605</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -6701,7 +6701,7 @@
         <v>1457</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>1652</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -6721,7 +6721,7 @@
         <v>1461</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>1656</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -6741,7 +6741,7 @@
         <v>1470</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>1665</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -6761,7 +6761,7 @@
         <v>1401</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>1597</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -6781,7 +6781,7 @@
         <v>1369</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>1566</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -6801,7 +6801,7 @@
         <v>1418</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>1614</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -6821,7 +6821,7 @@
         <v>1381</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>1578</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -6841,7 +6841,7 @@
         <v>1468</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>1663</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -6861,7 +6861,7 @@
         <v>1384</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>1580</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -6881,7 +6881,7 @@
         <v>1488</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>1683</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -6901,7 +6901,7 @@
         <v>1421</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>1617</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -6921,7 +6921,7 @@
         <v>1367</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>1564</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -6941,7 +6941,7 @@
         <v>1392</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>1588</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -6961,7 +6961,7 @@
         <v>1359</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>1556</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -6981,7 +6981,7 @@
         <v>1489</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>1684</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -7001,7 +7001,7 @@
         <v>1485</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>1680</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -7021,7 +7021,7 @@
         <v>1365</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>1562</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -7041,7 +7041,7 @@
         <v>1481</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>1676</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
@@ -7061,7 +7061,7 @@
         <v>1435</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>1630</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -7081,7 +7081,7 @@
         <v>1482</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>1677</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -7101,7 +7101,7 @@
         <v>1517</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
@@ -7121,7 +7121,7 @@
         <v>1354</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>1551</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -7141,7 +7141,7 @@
         <v>1415</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>1611</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -7161,7 +7161,7 @@
         <v>1417</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>1613</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -7181,7 +7181,7 @@
         <v>1505</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>1700</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -7201,7 +7201,7 @@
         <v>1386</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>1582</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
@@ -7221,7 +7221,7 @@
         <v>1467</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>1662</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -7241,7 +7241,7 @@
         <v>1351</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>1548</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -7261,7 +7261,7 @@
         <v>1449</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>1644</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
@@ -7281,7 +7281,7 @@
         <v>1366</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>1563</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
@@ -7301,7 +7301,7 @@
         <v>1439</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>1634</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -7321,7 +7321,7 @@
         <v>1375</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>1572</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
@@ -7341,7 +7341,7 @@
         <v>1518</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>1546</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -7361,7 +7361,7 @@
         <v>1427</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>1623</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -7381,7 +7381,7 @@
         <v>1376</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>1573</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
@@ -7401,7 +7401,7 @@
         <v>1498</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>1693</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -7421,7 +7421,7 @@
         <v>1473</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>1668</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -7441,7 +7441,7 @@
         <v>1513</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>1708</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
@@ -7461,7 +7461,7 @@
         <v>1499</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>1694</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -7481,7 +7481,7 @@
         <v>1416</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>1612</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -7501,7 +7501,7 @@
         <v>1474</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>1669</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
@@ -7521,7 +7521,7 @@
         <v>1388</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>1584</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -7541,7 +7541,7 @@
         <v>1430</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>1626</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -7561,7 +7561,7 @@
         <v>1355</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>1552</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -7581,7 +7581,7 @@
         <v>1399</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>1595</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -7601,7 +7601,7 @@
         <v>1471</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>1666</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
@@ -7621,7 +7621,7 @@
         <v>1432</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>1628</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -7641,7 +7641,7 @@
         <v>1363</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>1560</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -7661,7 +7661,7 @@
         <v>1483</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>1678</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -7681,7 +7681,7 @@
         <v>1475</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>1670</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -7701,7 +7701,7 @@
         <v>1387</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>1583</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -7721,7 +7721,7 @@
         <v>1486</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>1681</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -7741,7 +7741,7 @@
         <v>1522</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>1712</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -7761,7 +7761,7 @@
         <v>1525</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>1726</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -7781,7 +7781,7 @@
         <v>1509</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>1704</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -7801,7 +7801,7 @@
         <v>1530</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>1727</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -7821,7 +7821,7 @@
         <v>1539</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>1728</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -7841,7 +7841,7 @@
         <v>1527</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>1716</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -7861,7 +7861,7 @@
         <v>1537</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>1729</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -7881,7 +7881,7 @@
         <v>1390</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>1586</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -7901,7 +7901,7 @@
         <v>1447</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>1642</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -7921,7 +7921,7 @@
         <v>1385</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>1581</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -7941,7 +7941,7 @@
         <v>1396</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>1592</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -7961,7 +7961,7 @@
         <v>1368</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>1565</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -7981,7 +7981,7 @@
         <v>1493</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>1688</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -8001,7 +8001,7 @@
         <v>1434</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>1730</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -8021,7 +8021,7 @@
         <v>1389</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>1585</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -8041,7 +8041,7 @@
         <v>1515</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>1543</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -8061,7 +8061,7 @@
         <v>1460</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>1655</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -8081,7 +8081,7 @@
         <v>1429</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>1625</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -8101,7 +8101,7 @@
         <v>1400</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>1596</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -8121,7 +8121,7 @@
         <v>1507</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>1702</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -8141,7 +8141,7 @@
         <v>1371</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>1568</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -8161,7 +8161,7 @@
         <v>1476</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>1671</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -8181,7 +8181,7 @@
         <v>1452</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>1647</v>
+        <v>1683</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -8201,7 +8201,7 @@
         <v>1451</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>1646</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -8221,7 +8221,7 @@
         <v>1357</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>1554</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -8241,7 +8241,7 @@
         <v>1516</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -8261,7 +8261,7 @@
         <v>1411</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>1607</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -8281,7 +8281,7 @@
         <v>1395</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>1591</v>
+        <v>1685</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -8301,7 +8301,7 @@
         <v>1520</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>1711</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -8341,7 +8341,7 @@
         <v>1533</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>1719</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -8361,7 +8361,7 @@
         <v>1542</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>1732</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -8381,7 +8381,7 @@
         <v>1454</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>1649</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -8401,7 +8401,7 @@
         <v>1479</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>1674</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -8421,7 +8421,7 @@
         <v>1450</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>1645</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -8441,7 +8441,7 @@
         <v>1442</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>1637</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -8461,7 +8461,7 @@
         <v>1487</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>1682</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -8481,7 +8481,7 @@
         <v>1441</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>1636</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -8501,7 +8501,7 @@
         <v>1491</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>1686</v>
+        <v>1689</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -8521,7 +8521,7 @@
         <v>1492</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>1687</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
@@ -8541,7 +8541,7 @@
         <v>1464</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>1659</v>
+        <v>1691</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
@@ -8561,7 +8561,7 @@
         <v>1407</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>1603</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
@@ -8581,7 +8581,7 @@
         <v>1405</v>
       </c>
       <c r="F145" s="3" t="s">
-        <v>1601</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
@@ -8601,7 +8601,7 @@
         <v>1455</v>
       </c>
       <c r="F146" s="3" t="s">
-        <v>1650</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
@@ -8621,7 +8621,7 @@
         <v>1445</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>1640</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
@@ -8641,7 +8641,7 @@
         <v>1469</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>1664</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
@@ -8661,7 +8661,7 @@
         <v>1437</v>
       </c>
       <c r="F149" s="3" t="s">
-        <v>1632</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
@@ -8681,7 +8681,7 @@
         <v>1459</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>1654</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
@@ -8701,7 +8701,7 @@
         <v>1352</v>
       </c>
       <c r="F151" s="3" t="s">
-        <v>1549</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
@@ -8721,7 +8721,7 @@
         <v>1511</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>1706</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
@@ -8741,7 +8741,7 @@
         <v>1403</v>
       </c>
       <c r="F153" s="3" t="s">
-        <v>1599</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
@@ -8761,7 +8761,7 @@
         <v>1506</v>
       </c>
       <c r="F154" s="3" t="s">
-        <v>1701</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
@@ -8781,7 +8781,7 @@
         <v>1494</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>1689</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
@@ -8801,7 +8801,7 @@
         <v>1438</v>
       </c>
       <c r="F156" s="3" t="s">
-        <v>1633</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
@@ -8821,7 +8821,7 @@
         <v>1410</v>
       </c>
       <c r="F157" s="3" t="s">
-        <v>1606</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
@@ -8841,7 +8841,7 @@
         <v>1472</v>
       </c>
       <c r="F158" s="3" t="s">
-        <v>1667</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
@@ -8861,7 +8861,7 @@
         <v>1413</v>
       </c>
       <c r="F159" s="3" t="s">
-        <v>1609</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
@@ -8881,7 +8881,7 @@
         <v>1521</v>
       </c>
       <c r="F160" s="3" t="s">
-        <v>1733</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
@@ -8921,7 +8921,7 @@
         <v>1446</v>
       </c>
       <c r="F162" s="3" t="s">
-        <v>1641</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
@@ -8941,7 +8941,7 @@
         <v>1436</v>
       </c>
       <c r="F163" s="3" t="s">
-        <v>1631</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.3">
@@ -8961,7 +8961,7 @@
         <v>1372</v>
       </c>
       <c r="F164" s="3" t="s">
-        <v>1569</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.3">
@@ -8981,7 +8981,7 @@
         <v>1398</v>
       </c>
       <c r="F165" s="3" t="s">
-        <v>1594</v>
+        <v>1704</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.3">
@@ -9001,7 +9001,7 @@
         <v>1443</v>
       </c>
       <c r="F166" s="3" t="s">
-        <v>1638</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.3">
@@ -9021,7 +9021,7 @@
         <v>1503</v>
       </c>
       <c r="F167" s="3" t="s">
-        <v>1698</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.3">
@@ -9041,7 +9041,7 @@
         <v>1370</v>
       </c>
       <c r="F168" s="3" t="s">
-        <v>1567</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.3">
@@ -9061,7 +9061,7 @@
         <v>1433</v>
       </c>
       <c r="F169" s="3" t="s">
-        <v>1629</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.3">
@@ -9081,7 +9081,7 @@
         <v>1453</v>
       </c>
       <c r="F170" s="3" t="s">
-        <v>1648</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.3">
@@ -9101,7 +9101,7 @@
         <v>1358</v>
       </c>
       <c r="F171" s="3" t="s">
-        <v>1555</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.3">
@@ -9121,7 +9121,7 @@
         <v>1402</v>
       </c>
       <c r="F172" s="3" t="s">
-        <v>1598</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.3">
@@ -9141,7 +9141,7 @@
         <v>1364</v>
       </c>
       <c r="F173" s="3" t="s">
-        <v>1561</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.3">
@@ -9161,7 +9161,7 @@
         <v>1510</v>
       </c>
       <c r="F174" s="3" t="s">
-        <v>1705</v>
+        <v>1708</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.3">
@@ -9181,7 +9181,7 @@
         <v>1377</v>
       </c>
       <c r="F175" s="3" t="s">
-        <v>1574</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.3">
@@ -9201,7 +9201,7 @@
         <v>1431</v>
       </c>
       <c r="F176" s="3" t="s">
-        <v>1627</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.3">
@@ -9221,7 +9221,7 @@
         <v>1490</v>
       </c>
       <c r="F177" s="3" t="s">
-        <v>1685</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.3">
@@ -9241,7 +9241,7 @@
         <v>1378</v>
       </c>
       <c r="F178" s="3" t="s">
-        <v>1575</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.3">
@@ -9261,7 +9261,7 @@
         <v>1440</v>
       </c>
       <c r="F179" s="3" t="s">
-        <v>1635</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.3">
@@ -9281,7 +9281,7 @@
         <v>1424</v>
       </c>
       <c r="F180" s="3" t="s">
-        <v>1620</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.3">
@@ -9301,7 +9301,7 @@
         <v>1382</v>
       </c>
       <c r="F181" s="3" t="s">
-        <v>1579</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.3">
@@ -9321,7 +9321,7 @@
         <v>1406</v>
       </c>
       <c r="F182" s="3" t="s">
-        <v>1602</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.3">
@@ -9341,7 +9341,7 @@
         <v>1383</v>
       </c>
       <c r="F183" s="3" t="s">
-        <v>1735</v>
+        <v>1728</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.3">
@@ -9361,7 +9361,7 @@
         <v>1361</v>
       </c>
       <c r="F184" s="3" t="s">
-        <v>1558</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.3">
@@ -9381,7 +9381,7 @@
         <v>1374</v>
       </c>
       <c r="F185" s="3" t="s">
-        <v>1571</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="186" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
@@ -9401,7 +9401,7 @@
         <v>1448</v>
       </c>
       <c r="F186" s="3" t="s">
-        <v>1643</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
@@ -9421,7 +9421,7 @@
         <v>1412</v>
       </c>
       <c r="F187" s="3" t="s">
-        <v>1608</v>
+        <v>1717</v>
       </c>
     </row>
     <row r="188" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
@@ -9441,7 +9441,7 @@
         <v>1393</v>
       </c>
       <c r="F188" s="3" t="s">
-        <v>1589</v>
+        <v>1718</v>
       </c>
     </row>
     <row r="189" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
@@ -9461,7 +9461,7 @@
         <v>1373</v>
       </c>
       <c r="F189" s="3" t="s">
-        <v>1570</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.3">
@@ -9481,7 +9481,7 @@
         <v>1353</v>
       </c>
       <c r="F190" s="3" t="s">
-        <v>1550</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="191" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
@@ -9501,7 +9501,7 @@
         <v>1422</v>
       </c>
       <c r="F191" s="3" t="s">
-        <v>1618</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="192" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
@@ -9521,7 +9521,7 @@
         <v>1458</v>
       </c>
       <c r="F192" s="3" t="s">
-        <v>1653</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="193" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
@@ -9541,7 +9541,7 @@
         <v>1501</v>
       </c>
       <c r="F193" s="3" t="s">
-        <v>1696</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.3">
@@ -9561,7 +9561,7 @@
         <v>1444</v>
       </c>
       <c r="F194" s="3" t="s">
-        <v>1639</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fixing space in name
</commit_message>
<xml_diff>
--- a/File Naming.xlsx
+++ b/File Naming.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\curly\Desktop\Apple Genotyping\Methods\Renaming Sample Labels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\curly\Desktop\Apple Genotyping\Methods\Renaming File Names\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C7067B-57B6-4709-8455-466557CC75CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53ACB88D-E72A-41D5-AEB4-5356511FC7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23040" yWindow="4440" windowWidth="23040" windowHeight="12120" xr2:uid="{3491D669-C83C-4979-B15B-06B44BE9C919}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{3491D669-C83C-4979-B15B-06B44BE9C919}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -4721,9 +4721,6 @@
     <t>Blakeway.CEL</t>
   </si>
   <si>
-    <t>Adam's Pearmain.CEL</t>
-  </si>
-  <si>
     <t>Fairbelle.CEL</t>
   </si>
   <si>
@@ -5309,12 +5306,6 @@
     <t>Abas.nexus.cnv.txt</t>
   </si>
   <si>
-    <t>Adam's Pearmain.txt</t>
-  </si>
-  <si>
-    <t>Adam's Pearmain.nexus.cnv.txt</t>
-  </si>
-  <si>
     <t>Akane.txt</t>
   </si>
   <si>
@@ -6396,6 +6387,15 @@
   </si>
   <si>
     <t>Karmijn_de_Sonnaville.nexus.cnv.txt</t>
+  </si>
+  <si>
+    <t>Adam's_Pearmain.CEL</t>
+  </si>
+  <si>
+    <t>Adam's_Pearmain.txt</t>
+  </si>
+  <si>
+    <t>Adam's_Pearmain.nexus.cnv.txt</t>
   </si>
 </sst>
 </file>
@@ -6824,8 +6824,8 @@
   <dimension ref="A1:F530"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A410" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D427" sqref="D427"/>
+      <pane ySplit="1" topLeftCell="A344" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D351" sqref="D351"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6839,10 +6839,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>672</v>
@@ -11754,13 +11754,13 @@
         <v>1520</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="C338" s="2" t="s">
+        <v>1730</v>
+      </c>
+      <c r="D338" s="2" t="s">
         <v>1731</v>
-      </c>
-      <c r="D338" s="2" t="s">
-        <v>1732</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.3">
@@ -11768,13 +11768,13 @@
         <v>1527</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="C339" s="2" t="s">
+        <v>1732</v>
+      </c>
+      <c r="D339" s="2" t="s">
         <v>1733</v>
-      </c>
-      <c r="D339" s="2" t="s">
-        <v>1734</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.3">
@@ -11782,13 +11782,13 @@
         <v>1519</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="C340" s="2" t="s">
+        <v>1734</v>
+      </c>
+      <c r="D340" s="2" t="s">
         <v>1735</v>
-      </c>
-      <c r="D340" s="2" t="s">
-        <v>1736</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.3">
@@ -11796,13 +11796,13 @@
         <v>1531</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="C341" s="2" t="s">
+        <v>1736</v>
+      </c>
+      <c r="D341" s="2" t="s">
         <v>1737</v>
-      </c>
-      <c r="D341" s="2" t="s">
-        <v>1738</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.3">
@@ -11810,13 +11810,13 @@
         <v>1528</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="C342" s="2" t="s">
+        <v>1738</v>
+      </c>
+      <c r="D342" s="2" t="s">
         <v>1739</v>
-      </c>
-      <c r="D342" s="2" t="s">
-        <v>1740</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.3">
@@ -11824,13 +11824,13 @@
         <v>1537</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="C343" s="2" t="s">
+        <v>1740</v>
+      </c>
+      <c r="D343" s="2" t="s">
         <v>1741</v>
-      </c>
-      <c r="D343" s="2" t="s">
-        <v>1742</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.3">
@@ -11838,13 +11838,13 @@
         <v>1515</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="C344" s="2" t="s">
+        <v>1742</v>
+      </c>
+      <c r="D344" s="2" t="s">
         <v>1743</v>
-      </c>
-      <c r="D344" s="2" t="s">
-        <v>1744</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.3">
@@ -11852,13 +11852,13 @@
         <v>1534</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="C345" s="2" t="s">
+        <v>1744</v>
+      </c>
+      <c r="D345" s="2" t="s">
         <v>1745</v>
-      </c>
-      <c r="D345" s="2" t="s">
-        <v>1746</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.3">
@@ -11866,13 +11866,13 @@
         <v>1525</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="C346" s="2" t="s">
+        <v>1746</v>
+      </c>
+      <c r="D346" s="2" t="s">
         <v>1747</v>
-      </c>
-      <c r="D346" s="2" t="s">
-        <v>1748</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.3">
@@ -11880,13 +11880,13 @@
         <v>1532</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="C347" s="2" t="s">
+        <v>1748</v>
+      </c>
+      <c r="D347" s="2" t="s">
         <v>1749</v>
-      </c>
-      <c r="D347" s="2" t="s">
-        <v>1750</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.3">
@@ -11894,13 +11894,13 @@
         <v>1522</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="C348" s="2" t="s">
+        <v>1750</v>
+      </c>
+      <c r="D348" s="2" t="s">
         <v>1751</v>
-      </c>
-      <c r="D348" s="2" t="s">
-        <v>1752</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.3">
@@ -11908,13 +11908,13 @@
         <v>1530</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="C349" s="2" t="s">
+        <v>1752</v>
+      </c>
+      <c r="D349" s="2" t="s">
         <v>1753</v>
-      </c>
-      <c r="D349" s="2" t="s">
-        <v>1754</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.3">
@@ -11925,10 +11925,10 @@
         <v>1541</v>
       </c>
       <c r="C350" s="2" t="s">
+        <v>1754</v>
+      </c>
+      <c r="D350" s="2" t="s">
         <v>1755</v>
-      </c>
-      <c r="D350" s="2" t="s">
-        <v>1756</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.3">
@@ -11936,13 +11936,13 @@
         <v>1416</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>1561</v>
+        <v>2117</v>
       </c>
       <c r="C351" s="2" t="s">
-        <v>1757</v>
+        <v>2118</v>
       </c>
       <c r="D351" s="2" t="s">
-        <v>1758</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.3">
@@ -11950,13 +11950,13 @@
         <v>1510</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="C352" s="2" t="s">
-        <v>1759</v>
+        <v>1756</v>
       </c>
       <c r="D352" s="2" t="s">
-        <v>1760</v>
+        <v>1757</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.3">
@@ -11964,13 +11964,13 @@
         <v>1458</v>
       </c>
       <c r="B353" s="3" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="C353" s="2" t="s">
-        <v>1761</v>
+        <v>1758</v>
       </c>
       <c r="D353" s="2" t="s">
-        <v>1762</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.3">
@@ -11978,13 +11978,13 @@
         <v>1474</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="C354" s="2" t="s">
-        <v>1763</v>
+        <v>1760</v>
       </c>
       <c r="D354" s="2" t="s">
-        <v>1764</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.3">
@@ -11992,13 +11992,13 @@
         <v>1508</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="C355" s="2" t="s">
-        <v>1765</v>
+        <v>1762</v>
       </c>
       <c r="D355" s="2" t="s">
-        <v>1766</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.3">
@@ -12006,13 +12006,13 @@
         <v>1480</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="C356" s="2" t="s">
-        <v>1767</v>
+        <v>1764</v>
       </c>
       <c r="D356" s="2" t="s">
-        <v>1768</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.3">
@@ -12020,13 +12020,13 @@
         <v>1410</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="C357" s="2" t="s">
-        <v>1769</v>
+        <v>1766</v>
       </c>
       <c r="D357" s="2" t="s">
-        <v>1770</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.3">
@@ -12034,13 +12034,13 @@
         <v>1358</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="C358" s="2" t="s">
-        <v>1771</v>
+        <v>1768</v>
       </c>
       <c r="D358" s="2" t="s">
-        <v>1772</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.3">
@@ -12051,10 +12051,10 @@
         <v>1550</v>
       </c>
       <c r="C359" s="2" t="s">
-        <v>1773</v>
+        <v>1770</v>
       </c>
       <c r="D359" s="2" t="s">
-        <v>1774</v>
+        <v>1771</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.3">
@@ -12062,13 +12062,13 @@
         <v>1421</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="C360" s="2" t="s">
-        <v>1775</v>
+        <v>1772</v>
       </c>
       <c r="D360" s="2" t="s">
-        <v>1776</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.3">
@@ -12076,13 +12076,13 @@
         <v>1422</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="C361" s="2" t="s">
-        <v>1777</v>
+        <v>1774</v>
       </c>
       <c r="D361" s="2" t="s">
-        <v>1778</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.3">
@@ -12090,13 +12090,13 @@
         <v>1452</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="C362" s="2" t="s">
-        <v>1779</v>
+        <v>1776</v>
       </c>
       <c r="D362" s="2" t="s">
-        <v>1780</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.3">
@@ -12104,13 +12104,13 @@
         <v>1462</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="C363" s="2" t="s">
-        <v>1781</v>
+        <v>1778</v>
       </c>
       <c r="D363" s="2" t="s">
-        <v>1782</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.3">
@@ -12118,13 +12118,13 @@
         <v>1390</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="C364" s="2" t="s">
-        <v>1783</v>
+        <v>1780</v>
       </c>
       <c r="D364" s="2" t="s">
-        <v>1784</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.3">
@@ -12132,13 +12132,13 @@
         <v>1356</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="C365" s="2" t="s">
-        <v>1785</v>
+        <v>1782</v>
       </c>
       <c r="D365" s="2" t="s">
-        <v>1786</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.3">
@@ -12146,13 +12146,13 @@
         <v>1498</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="C366" s="2" t="s">
-        <v>1787</v>
+        <v>1784</v>
       </c>
       <c r="D366" s="2" t="s">
-        <v>1788</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.3">
@@ -12160,13 +12160,13 @@
         <v>1476</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="C367" s="2" t="s">
-        <v>1789</v>
+        <v>1786</v>
       </c>
       <c r="D367" s="2" t="s">
-        <v>1790</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.3">
@@ -12174,13 +12174,13 @@
         <v>1492</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="C368" s="2" t="s">
-        <v>1791</v>
+        <v>1788</v>
       </c>
       <c r="D368" s="2" t="s">
-        <v>1792</v>
+        <v>1789</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.3">
@@ -12188,13 +12188,13 @@
         <v>1461</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="C369" s="2" t="s">
-        <v>1793</v>
+        <v>1790</v>
       </c>
       <c r="D369" s="2" t="s">
-        <v>1794</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.3">
@@ -12205,10 +12205,10 @@
         <v>1560</v>
       </c>
       <c r="C370" s="2" t="s">
-        <v>1795</v>
+        <v>1792</v>
       </c>
       <c r="D370" s="2" t="s">
-        <v>1796</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.3">
@@ -12216,13 +12216,13 @@
         <v>1424</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="C371" s="2" t="s">
-        <v>1797</v>
+        <v>1794</v>
       </c>
       <c r="D371" s="2" t="s">
-        <v>1798</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.3">
@@ -12230,13 +12230,13 @@
         <v>1491</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="C372" s="2" t="s">
-        <v>1799</v>
+        <v>1796</v>
       </c>
       <c r="D372" s="2" t="s">
-        <v>1800</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.3">
@@ -12244,13 +12244,13 @@
         <v>1473</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="C373" s="2" t="s">
-        <v>1801</v>
+        <v>1798</v>
       </c>
       <c r="D373" s="2" t="s">
-        <v>1802</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.3">
@@ -12258,13 +12258,13 @@
         <v>1500</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="C374" s="2" t="s">
-        <v>1803</v>
+        <v>1800</v>
       </c>
       <c r="D374" s="2" t="s">
-        <v>1804</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.3">
@@ -12272,13 +12272,13 @@
         <v>1419</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="C375" s="2" t="s">
-        <v>1805</v>
+        <v>1802</v>
       </c>
       <c r="D375" s="2" t="s">
-        <v>1806</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.3">
@@ -12286,13 +12286,13 @@
         <v>1393</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="C376" s="2" t="s">
-        <v>1807</v>
+        <v>1804</v>
       </c>
       <c r="D376" s="2" t="s">
-        <v>1808</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.3">
@@ -12303,10 +12303,10 @@
         <v>1555</v>
       </c>
       <c r="C377" s="2" t="s">
-        <v>1809</v>
+        <v>1806</v>
       </c>
       <c r="D377" s="2" t="s">
-        <v>1810</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.3">
@@ -12314,13 +12314,13 @@
         <v>1387</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="C378" s="2" t="s">
-        <v>1811</v>
+        <v>1808</v>
       </c>
       <c r="D378" s="2" t="s">
-        <v>1812</v>
+        <v>1809</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.3">
@@ -12328,13 +12328,13 @@
         <v>1352</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="C379" s="2" t="s">
-        <v>1813</v>
+        <v>1810</v>
       </c>
       <c r="D379" s="2" t="s">
-        <v>1814</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.3">
@@ -12342,13 +12342,13 @@
         <v>1400</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="C380" s="2" t="s">
-        <v>1815</v>
+        <v>1812</v>
       </c>
       <c r="D380" s="2" t="s">
-        <v>1816</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.3">
@@ -12359,10 +12359,10 @@
         <v>1549</v>
       </c>
       <c r="C381" s="2" t="s">
-        <v>1817</v>
+        <v>1814</v>
       </c>
       <c r="D381" s="2" t="s">
-        <v>1818</v>
+        <v>1815</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.3">
@@ -12370,13 +12370,13 @@
         <v>1504</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="C382" s="2" t="s">
-        <v>1819</v>
+        <v>1816</v>
       </c>
       <c r="D382" s="2" t="s">
-        <v>1820</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.3">
@@ -12384,13 +12384,13 @@
         <v>1493</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="C383" s="2" t="s">
-        <v>1821</v>
+        <v>1818</v>
       </c>
       <c r="D383" s="2" t="s">
-        <v>1822</v>
+        <v>1819</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.3">
@@ -12398,13 +12398,13 @@
         <v>1496</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="C384" s="2" t="s">
-        <v>1823</v>
+        <v>1820</v>
       </c>
       <c r="D384" s="2" t="s">
-        <v>1824</v>
+        <v>1821</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.3">
@@ -12412,13 +12412,13 @@
         <v>1459</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="C385" s="2" t="s">
-        <v>1825</v>
+        <v>1822</v>
       </c>
       <c r="D385" s="2" t="s">
-        <v>1826</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.3">
@@ -12429,10 +12429,10 @@
         <v>1556</v>
       </c>
       <c r="C386" s="2" t="s">
-        <v>1827</v>
+        <v>1824</v>
       </c>
       <c r="D386" s="2" t="s">
-        <v>1828</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.3">
@@ -12440,13 +12440,13 @@
         <v>1453</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="C387" s="2" t="s">
-        <v>1829</v>
+        <v>1826</v>
       </c>
       <c r="D387" s="2" t="s">
-        <v>1830</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.3">
@@ -12454,13 +12454,13 @@
         <v>1457</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="C388" s="2" t="s">
-        <v>1831</v>
+        <v>1828</v>
       </c>
       <c r="D388" s="2" t="s">
-        <v>1832</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.3">
@@ -12468,13 +12468,13 @@
         <v>1466</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="C389" s="2" t="s">
-        <v>1833</v>
+        <v>1830</v>
       </c>
       <c r="D389" s="2" t="s">
-        <v>1834</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.3">
@@ -12485,10 +12485,10 @@
         <v>1552</v>
       </c>
       <c r="C390" s="2" t="s">
-        <v>1835</v>
+        <v>1832</v>
       </c>
       <c r="D390" s="2" t="s">
-        <v>1836</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.3">
@@ -12499,10 +12499,10 @@
         <v>1545</v>
       </c>
       <c r="C391" s="2" t="s">
-        <v>1837</v>
+        <v>1834</v>
       </c>
       <c r="D391" s="2" t="s">
-        <v>1838</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.3">
@@ -12513,10 +12513,10 @@
         <v>1559</v>
       </c>
       <c r="C392" s="2" t="s">
-        <v>1839</v>
+        <v>1836</v>
       </c>
       <c r="D392" s="2" t="s">
-        <v>1840</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.3">
@@ -12524,13 +12524,13 @@
         <v>1377</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="C393" s="2" t="s">
-        <v>1841</v>
+        <v>1838</v>
       </c>
       <c r="D393" s="2" t="s">
-        <v>1842</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.3">
@@ -12538,13 +12538,13 @@
         <v>1464</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="C394" s="2" t="s">
-        <v>1843</v>
+        <v>1840</v>
       </c>
       <c r="D394" s="2" t="s">
-        <v>1844</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.3">
@@ -12552,13 +12552,13 @@
         <v>1380</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="C395" s="2" t="s">
-        <v>1845</v>
+        <v>1842</v>
       </c>
       <c r="D395" s="2" t="s">
-        <v>1846</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.3">
@@ -12566,13 +12566,13 @@
         <v>1484</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="C396" s="2" t="s">
-        <v>1847</v>
+        <v>1844</v>
       </c>
       <c r="D396" s="2" t="s">
-        <v>1848</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.3">
@@ -12580,13 +12580,13 @@
         <v>1417</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="C397" s="2" t="s">
-        <v>1849</v>
+        <v>1846</v>
       </c>
       <c r="D397" s="2" t="s">
-        <v>1850</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.3">
@@ -12594,13 +12594,13 @@
         <v>1363</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="C398" s="2" t="s">
-        <v>1851</v>
+        <v>1848</v>
       </c>
       <c r="D398" s="2" t="s">
-        <v>1852</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.3">
@@ -12608,13 +12608,13 @@
         <v>1388</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="C399" s="2" t="s">
-        <v>1853</v>
+        <v>1850</v>
       </c>
       <c r="D399" s="2" t="s">
-        <v>1854</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.3">
@@ -12622,13 +12622,13 @@
         <v>1355</v>
       </c>
       <c r="B400" s="3" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="C400" s="2" t="s">
-        <v>1855</v>
+        <v>1852</v>
       </c>
       <c r="D400" s="2" t="s">
-        <v>1856</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.3">
@@ -12636,13 +12636,13 @@
         <v>1485</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="C401" s="2" t="s">
-        <v>1857</v>
+        <v>1854</v>
       </c>
       <c r="D401" s="2" t="s">
-        <v>1858</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.3">
@@ -12650,13 +12650,13 @@
         <v>1481</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="C402" s="2" t="s">
-        <v>1859</v>
+        <v>1856</v>
       </c>
       <c r="D402" s="2" t="s">
-        <v>1860</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.3">
@@ -12664,13 +12664,13 @@
         <v>1361</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="C403" s="2" t="s">
-        <v>1861</v>
+        <v>1858</v>
       </c>
       <c r="D403" s="2" t="s">
-        <v>1862</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.3">
@@ -12678,13 +12678,13 @@
         <v>1477</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="C404" s="2" t="s">
-        <v>1863</v>
+        <v>1860</v>
       </c>
       <c r="D404" s="2" t="s">
-        <v>1864</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.3">
@@ -12692,13 +12692,13 @@
         <v>1431</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="C405" s="2" t="s">
-        <v>1865</v>
+        <v>1862</v>
       </c>
       <c r="D405" s="2" t="s">
-        <v>1866</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.3">
@@ -12706,13 +12706,13 @@
         <v>1478</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="C406" s="2" t="s">
-        <v>1867</v>
+        <v>1864</v>
       </c>
       <c r="D406" s="2" t="s">
-        <v>1868</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.3">
@@ -12723,10 +12723,10 @@
         <v>1540</v>
       </c>
       <c r="C407" s="2" t="s">
-        <v>1869</v>
+        <v>1866</v>
       </c>
       <c r="D407" s="2" t="s">
-        <v>1870</v>
+        <v>1867</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.3">
@@ -12734,13 +12734,13 @@
         <v>1350</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="C408" s="2" t="s">
-        <v>1871</v>
+        <v>1868</v>
       </c>
       <c r="D408" s="2" t="s">
-        <v>1872</v>
+        <v>1869</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.3">
@@ -12748,13 +12748,13 @@
         <v>1411</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="C409" s="2" t="s">
-        <v>1873</v>
+        <v>1870</v>
       </c>
       <c r="D409" s="2" t="s">
-        <v>1874</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.3">
@@ -12762,13 +12762,13 @@
         <v>1413</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="C410" s="2" t="s">
-        <v>1875</v>
+        <v>1872</v>
       </c>
       <c r="D410" s="2" t="s">
-        <v>1876</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.3">
@@ -12776,13 +12776,13 @@
         <v>1501</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="C411" s="2" t="s">
-        <v>1877</v>
+        <v>1874</v>
       </c>
       <c r="D411" s="2" t="s">
-        <v>1878</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.3">
@@ -12790,13 +12790,13 @@
         <v>1382</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="C412" s="2" t="s">
-        <v>1879</v>
+        <v>1876</v>
       </c>
       <c r="D412" s="2" t="s">
-        <v>1880</v>
+        <v>1877</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.3">
@@ -12804,13 +12804,13 @@
         <v>1463</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="C413" s="2" t="s">
-        <v>1881</v>
+        <v>1878</v>
       </c>
       <c r="D413" s="2" t="s">
-        <v>1882</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.3">
@@ -12818,13 +12818,13 @@
         <v>1347</v>
       </c>
       <c r="B414" s="3" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="C414" s="2" t="s">
-        <v>1883</v>
+        <v>1880</v>
       </c>
       <c r="D414" s="2" t="s">
-        <v>1884</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.3">
@@ -12832,13 +12832,13 @@
         <v>1445</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="C415" s="2" t="s">
-        <v>1885</v>
+        <v>1882</v>
       </c>
       <c r="D415" s="2" t="s">
-        <v>1886</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.3">
@@ -12846,13 +12846,13 @@
         <v>1362</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="C416" s="2" t="s">
-        <v>1887</v>
+        <v>1884</v>
       </c>
       <c r="D416" s="2" t="s">
-        <v>1888</v>
+        <v>1885</v>
       </c>
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.3">
@@ -12860,13 +12860,13 @@
         <v>1435</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="C417" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="D417" s="2" t="s">
-        <v>1890</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.3">
@@ -12874,13 +12874,13 @@
         <v>1371</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="C418" s="2" t="s">
-        <v>1891</v>
+        <v>1888</v>
       </c>
       <c r="D418" s="2" t="s">
-        <v>1892</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.3">
@@ -12888,13 +12888,13 @@
         <v>1514</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="C419" s="2" t="s">
-        <v>1893</v>
+        <v>1890</v>
       </c>
       <c r="D419" s="2" t="s">
-        <v>1894</v>
+        <v>1891</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.3">
@@ -12902,13 +12902,13 @@
         <v>1423</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="C420" s="2" t="s">
-        <v>1895</v>
+        <v>1892</v>
       </c>
       <c r="D420" s="2" t="s">
-        <v>1896</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.3">
@@ -12919,10 +12919,10 @@
         <v>1547</v>
       </c>
       <c r="C421" s="2" t="s">
-        <v>1897</v>
+        <v>1894</v>
       </c>
       <c r="D421" s="2" t="s">
-        <v>1898</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.3">
@@ -12930,13 +12930,13 @@
         <v>1494</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="C422" s="2" t="s">
-        <v>1899</v>
+        <v>1896</v>
       </c>
       <c r="D422" s="2" t="s">
-        <v>1900</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.3">
@@ -12944,13 +12944,13 @@
         <v>1469</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="C423" s="2" t="s">
-        <v>1901</v>
+        <v>1898</v>
       </c>
       <c r="D423" s="2" t="s">
-        <v>1902</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.3">
@@ -12958,13 +12958,13 @@
         <v>1509</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="C424" s="2" t="s">
-        <v>1903</v>
+        <v>1900</v>
       </c>
       <c r="D424" s="2" t="s">
-        <v>1904</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.3">
@@ -12972,13 +12972,13 @@
         <v>1495</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="C425" s="2" t="s">
-        <v>1905</v>
+        <v>1902</v>
       </c>
       <c r="D425" s="2" t="s">
-        <v>1906</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.3">
@@ -12986,13 +12986,13 @@
         <v>1412</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="C426" s="2" t="s">
-        <v>1907</v>
+        <v>1904</v>
       </c>
       <c r="D426" s="2" t="s">
-        <v>1908</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.3">
@@ -13000,13 +13000,13 @@
         <v>1470</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>2117</v>
+        <v>2114</v>
       </c>
       <c r="C427" s="2" t="s">
-        <v>2118</v>
+        <v>2115</v>
       </c>
       <c r="D427" s="2" t="s">
-        <v>2119</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.3">
@@ -13014,13 +13014,13 @@
         <v>1384</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="C428" s="2" t="s">
-        <v>1909</v>
+        <v>1906</v>
       </c>
       <c r="D428" s="2" t="s">
-        <v>1910</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.3">
@@ -13028,13 +13028,13 @@
         <v>1426</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="C429" s="2" t="s">
-        <v>1911</v>
+        <v>1908</v>
       </c>
       <c r="D429" s="2" t="s">
-        <v>1912</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.3">
@@ -13042,13 +13042,13 @@
         <v>1351</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="C430" s="2" t="s">
-        <v>1913</v>
+        <v>1910</v>
       </c>
       <c r="D430" s="2" t="s">
-        <v>1914</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.3">
@@ -13056,13 +13056,13 @@
         <v>1395</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="C431" s="2" t="s">
-        <v>1915</v>
+        <v>1912</v>
       </c>
       <c r="D431" s="2" t="s">
-        <v>1916</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.3">
@@ -13070,13 +13070,13 @@
         <v>1467</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="C432" s="2" t="s">
-        <v>1917</v>
+        <v>1914</v>
       </c>
       <c r="D432" s="2" t="s">
-        <v>1918</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.3">
@@ -13084,13 +13084,13 @@
         <v>1428</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="C433" s="2" t="s">
-        <v>1919</v>
+        <v>1916</v>
       </c>
       <c r="D433" s="2" t="s">
-        <v>1920</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.3">
@@ -13101,10 +13101,10 @@
         <v>1544</v>
       </c>
       <c r="C434" s="2" t="s">
-        <v>1921</v>
+        <v>1918</v>
       </c>
       <c r="D434" s="2" t="s">
-        <v>1922</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.3">
@@ -13112,13 +13112,13 @@
         <v>1479</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="C435" s="2" t="s">
-        <v>1923</v>
+        <v>1920</v>
       </c>
       <c r="D435" s="2" t="s">
-        <v>1924</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.3">
@@ -13126,13 +13126,13 @@
         <v>1471</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="C436" s="2" t="s">
-        <v>1925</v>
+        <v>1922</v>
       </c>
       <c r="D436" s="2" t="s">
-        <v>1926</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.3">
@@ -13140,13 +13140,13 @@
         <v>1383</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="C437" s="2" t="s">
-        <v>1927</v>
+        <v>1924</v>
       </c>
       <c r="D437" s="2" t="s">
-        <v>1928</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.3">
@@ -13154,13 +13154,13 @@
         <v>1482</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="C438" s="2" t="s">
-        <v>1929</v>
+        <v>1926</v>
       </c>
       <c r="D438" s="2" t="s">
-        <v>1930</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.3">
@@ -13168,13 +13168,13 @@
         <v>1518</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="C439" s="2" t="s">
-        <v>1931</v>
+        <v>1928</v>
       </c>
       <c r="D439" s="2" t="s">
-        <v>1932</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.3">
@@ -13182,13 +13182,13 @@
         <v>1521</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="C440" s="2" t="s">
-        <v>1933</v>
+        <v>1930</v>
       </c>
       <c r="D440" s="2" t="s">
-        <v>1934</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.3">
@@ -13196,13 +13196,13 @@
         <v>1505</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="C441" s="2" t="s">
-        <v>1935</v>
+        <v>1932</v>
       </c>
       <c r="D441" s="2" t="s">
-        <v>1936</v>
+        <v>1933</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.3">
@@ -13210,13 +13210,13 @@
         <v>1526</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="C442" s="2" t="s">
-        <v>1937</v>
+        <v>1934</v>
       </c>
       <c r="D442" s="2" t="s">
-        <v>1938</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.3">
@@ -13224,13 +13224,13 @@
         <v>1535</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="C443" s="2" t="s">
-        <v>1939</v>
+        <v>1936</v>
       </c>
       <c r="D443" s="2" t="s">
-        <v>1940</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.3">
@@ -13238,13 +13238,13 @@
         <v>1523</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="C444" s="2" t="s">
-        <v>1941</v>
+        <v>1938</v>
       </c>
       <c r="D444" s="2" t="s">
-        <v>1942</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.3">
@@ -13252,13 +13252,13 @@
         <v>1533</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="C445" s="2" t="s">
-        <v>1943</v>
+        <v>1940</v>
       </c>
       <c r="D445" s="2" t="s">
-        <v>1944</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.3">
@@ -13266,13 +13266,13 @@
         <v>1386</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="C446" s="2" t="s">
-        <v>1945</v>
+        <v>1942</v>
       </c>
       <c r="D446" s="2" t="s">
-        <v>1946</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.3">
@@ -13280,13 +13280,13 @@
         <v>1443</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="C447" s="2" t="s">
-        <v>1947</v>
+        <v>1944</v>
       </c>
       <c r="D447" s="2" t="s">
-        <v>1948</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.3">
@@ -13294,13 +13294,13 @@
         <v>1381</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="C448" s="2" t="s">
-        <v>1949</v>
+        <v>1946</v>
       </c>
       <c r="D448" s="2" t="s">
-        <v>1950</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.3">
@@ -13308,13 +13308,13 @@
         <v>1392</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="C449" s="2" t="s">
-        <v>1951</v>
+        <v>1948</v>
       </c>
       <c r="D449" s="2" t="s">
-        <v>1952</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.3">
@@ -13322,13 +13322,13 @@
         <v>1364</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="C450" s="2" t="s">
-        <v>1953</v>
+        <v>1950</v>
       </c>
       <c r="D450" s="2" t="s">
-        <v>1954</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.3">
@@ -13336,13 +13336,13 @@
         <v>1489</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="C451" s="2" t="s">
-        <v>1955</v>
+        <v>1952</v>
       </c>
       <c r="D451" s="2" t="s">
-        <v>1956</v>
+        <v>1953</v>
       </c>
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.3">
@@ -13350,13 +13350,13 @@
         <v>1430</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="C452" s="2" t="s">
-        <v>1957</v>
+        <v>1954</v>
       </c>
       <c r="D452" s="2" t="s">
-        <v>1958</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.3">
@@ -13367,10 +13367,10 @@
         <v>1551</v>
       </c>
       <c r="C453" s="2" t="s">
-        <v>1959</v>
+        <v>1956</v>
       </c>
       <c r="D453" s="2" t="s">
-        <v>1960</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.3">
@@ -13378,13 +13378,13 @@
         <v>1511</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="C454" s="2" t="s">
-        <v>1961</v>
+        <v>1958</v>
       </c>
       <c r="D454" s="2" t="s">
-        <v>1962</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.3">
@@ -13392,13 +13392,13 @@
         <v>1456</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="C455" s="2" t="s">
-        <v>1963</v>
+        <v>1960</v>
       </c>
       <c r="D455" s="2" t="s">
-        <v>1964</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.3">
@@ -13406,13 +13406,13 @@
         <v>1425</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="C456" s="2" t="s">
-        <v>1965</v>
+        <v>1962</v>
       </c>
       <c r="D456" s="2" t="s">
-        <v>1966</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.3">
@@ -13420,13 +13420,13 @@
         <v>1396</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="C457" s="2" t="s">
-        <v>1967</v>
+        <v>1964</v>
       </c>
       <c r="D457" s="2" t="s">
-        <v>1968</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.3">
@@ -13434,13 +13434,13 @@
         <v>1503</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="C458" s="2" t="s">
-        <v>1969</v>
+        <v>1966</v>
       </c>
       <c r="D458" s="2" t="s">
-        <v>1970</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.3">
@@ -13448,13 +13448,13 @@
         <v>1367</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="C459" s="2" t="s">
-        <v>1971</v>
+        <v>1968</v>
       </c>
       <c r="D459" s="2" t="s">
-        <v>1972</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.3">
@@ -13462,13 +13462,13 @@
         <v>1472</v>
       </c>
       <c r="B460" s="3" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="C460" s="2" t="s">
-        <v>1973</v>
+        <v>1970</v>
       </c>
       <c r="D460" s="2" t="s">
-        <v>1974</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.3">
@@ -13476,13 +13476,13 @@
         <v>1448</v>
       </c>
       <c r="B461" s="3" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
       <c r="C461" s="2" t="s">
-        <v>1975</v>
+        <v>1972</v>
       </c>
       <c r="D461" s="2" t="s">
-        <v>1976</v>
+        <v>1973</v>
       </c>
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.3">
@@ -13490,13 +13490,13 @@
         <v>1447</v>
       </c>
       <c r="B462" s="3" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="C462" s="2" t="s">
-        <v>1977</v>
+        <v>1974</v>
       </c>
       <c r="D462" s="2" t="s">
-        <v>1978</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.3">
@@ -13504,13 +13504,13 @@
         <v>1353</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="C463" s="2" t="s">
-        <v>1979</v>
+        <v>1976</v>
       </c>
       <c r="D463" s="2" t="s">
-        <v>1980</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="464" spans="1:4" x14ac:dyDescent="0.3">
@@ -13521,10 +13521,10 @@
         <v>1539</v>
       </c>
       <c r="C464" s="2" t="s">
-        <v>1981</v>
+        <v>1978</v>
       </c>
       <c r="D464" s="2" t="s">
-        <v>1982</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="465" spans="1:4" x14ac:dyDescent="0.3">
@@ -13535,10 +13535,10 @@
         <v>1557</v>
       </c>
       <c r="C465" s="2" t="s">
-        <v>1983</v>
+        <v>1980</v>
       </c>
       <c r="D465" s="2" t="s">
-        <v>1984</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="466" spans="1:4" x14ac:dyDescent="0.3">
@@ -13546,13 +13546,13 @@
         <v>1391</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="C466" s="2" t="s">
-        <v>1985</v>
+        <v>1982</v>
       </c>
       <c r="D466" s="2" t="s">
-        <v>1986</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="467" spans="1:4" x14ac:dyDescent="0.3">
@@ -13560,13 +13560,13 @@
         <v>1516</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="C467" s="2" t="s">
-        <v>1987</v>
+        <v>1984</v>
       </c>
       <c r="D467" s="2" t="s">
-        <v>1988</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="468" spans="1:4" x14ac:dyDescent="0.3">
@@ -13574,13 +13574,13 @@
         <v>1524</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="C468" s="2" t="s">
-        <v>1989</v>
+        <v>1986</v>
       </c>
       <c r="D468" s="2" t="s">
-        <v>1990</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="469" spans="1:4" x14ac:dyDescent="0.3">
@@ -13588,13 +13588,13 @@
         <v>1529</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="C469" s="2" t="s">
-        <v>1991</v>
+        <v>1988</v>
       </c>
       <c r="D469" s="2" t="s">
-        <v>1992</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.3">
@@ -13602,13 +13602,13 @@
         <v>1538</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="C470" s="2" t="s">
-        <v>1993</v>
+        <v>1990</v>
       </c>
       <c r="D470" s="2" t="s">
-        <v>1994</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.3">
@@ -13616,13 +13616,13 @@
         <v>1450</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="C471" s="2" t="s">
-        <v>1995</v>
+        <v>1992</v>
       </c>
       <c r="D471" s="2" t="s">
-        <v>1996</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="472" spans="1:4" x14ac:dyDescent="0.3">
@@ -13630,13 +13630,13 @@
         <v>1475</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="C472" s="2" t="s">
-        <v>1997</v>
+        <v>1994</v>
       </c>
       <c r="D472" s="2" t="s">
-        <v>1998</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="473" spans="1:4" x14ac:dyDescent="0.3">
@@ -13644,13 +13644,13 @@
         <v>1446</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="C473" s="2" t="s">
-        <v>1999</v>
+        <v>1996</v>
       </c>
       <c r="D473" s="2" t="s">
-        <v>2000</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="474" spans="1:4" x14ac:dyDescent="0.3">
@@ -13658,13 +13658,13 @@
         <v>1438</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="C474" s="2" t="s">
-        <v>2001</v>
+        <v>1998</v>
       </c>
       <c r="D474" s="2" t="s">
-        <v>2002</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="475" spans="1:4" x14ac:dyDescent="0.3">
@@ -13672,13 +13672,13 @@
         <v>1483</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="C475" s="2" t="s">
-        <v>2003</v>
+        <v>2000</v>
       </c>
       <c r="D475" s="2" t="s">
-        <v>2004</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="476" spans="1:4" x14ac:dyDescent="0.3">
@@ -13686,13 +13686,13 @@
         <v>1437</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="C476" s="2" t="s">
-        <v>2005</v>
+        <v>2002</v>
       </c>
       <c r="D476" s="2" t="s">
-        <v>2006</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="477" spans="1:4" x14ac:dyDescent="0.3">
@@ -13700,13 +13700,13 @@
         <v>1487</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="C477" s="2" t="s">
-        <v>2007</v>
+        <v>2004</v>
       </c>
       <c r="D477" s="2" t="s">
-        <v>2008</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="478" spans="1:4" x14ac:dyDescent="0.3">
@@ -13714,13 +13714,13 @@
         <v>1488</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="C478" s="2" t="s">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="D478" s="2" t="s">
-        <v>2010</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="479" spans="1:4" x14ac:dyDescent="0.3">
@@ -13728,13 +13728,13 @@
         <v>1460</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="C479" s="2" t="s">
-        <v>2011</v>
+        <v>2008</v>
       </c>
       <c r="D479" s="2" t="s">
-        <v>2012</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="480" spans="1:4" x14ac:dyDescent="0.3">
@@ -13742,13 +13742,13 @@
         <v>1403</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="C480" s="2" t="s">
-        <v>2013</v>
+        <v>2010</v>
       </c>
       <c r="D480" s="2" t="s">
-        <v>2014</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="481" spans="1:4" x14ac:dyDescent="0.3">
@@ -13756,13 +13756,13 @@
         <v>1401</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="C481" s="2" t="s">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="D481" s="2" t="s">
-        <v>2016</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="482" spans="1:4" x14ac:dyDescent="0.3">
@@ -13770,13 +13770,13 @@
         <v>1451</v>
       </c>
       <c r="B482" s="3" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="C482" s="2" t="s">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="D482" s="2" t="s">
-        <v>2018</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="483" spans="1:4" x14ac:dyDescent="0.3">
@@ -13784,13 +13784,13 @@
         <v>1441</v>
       </c>
       <c r="B483" s="3" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="C483" s="2" t="s">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="D483" s="2" t="s">
-        <v>2020</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="484" spans="1:4" x14ac:dyDescent="0.3">
@@ -13798,13 +13798,13 @@
         <v>1465</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="C484" s="2" t="s">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="D484" s="2" t="s">
-        <v>2022</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="485" spans="1:4" x14ac:dyDescent="0.3">
@@ -13812,13 +13812,13 @@
         <v>1433</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="C485" s="2" t="s">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="D485" s="2" t="s">
-        <v>2024</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="486" spans="1:4" x14ac:dyDescent="0.3">
@@ -13826,13 +13826,13 @@
         <v>1455</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="C486" s="2" t="s">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="D486" s="2" t="s">
-        <v>2026</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="487" spans="1:4" x14ac:dyDescent="0.3">
@@ -13843,10 +13843,10 @@
         <v>1542</v>
       </c>
       <c r="C487" s="2" t="s">
-        <v>2027</v>
+        <v>2024</v>
       </c>
       <c r="D487" s="2" t="s">
-        <v>2028</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.3">
@@ -13854,13 +13854,13 @@
         <v>1507</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="C488" s="2" t="s">
-        <v>2029</v>
+        <v>2026</v>
       </c>
       <c r="D488" s="2" t="s">
-        <v>2030</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.3">
@@ -13871,10 +13871,10 @@
         <v>1554</v>
       </c>
       <c r="C489" s="2" t="s">
-        <v>2031</v>
+        <v>2028</v>
       </c>
       <c r="D489" s="2" t="s">
-        <v>2032</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.3">
@@ -13882,13 +13882,13 @@
         <v>1502</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="C490" s="2" t="s">
-        <v>2033</v>
+        <v>2030</v>
       </c>
       <c r="D490" s="2" t="s">
-        <v>2034</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="491" spans="1:4" x14ac:dyDescent="0.3">
@@ -13896,13 +13896,13 @@
         <v>1490</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="C491" s="2" t="s">
-        <v>2035</v>
+        <v>2032</v>
       </c>
       <c r="D491" s="2" t="s">
-        <v>2036</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="492" spans="1:4" x14ac:dyDescent="0.3">
@@ -13910,13 +13910,13 @@
         <v>1434</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="C492" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="D492" s="2" t="s">
-        <v>2038</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="493" spans="1:4" x14ac:dyDescent="0.3">
@@ -13924,13 +13924,13 @@
         <v>1406</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="C493" s="2" t="s">
-        <v>2039</v>
+        <v>2036</v>
       </c>
       <c r="D493" s="2" t="s">
-        <v>2040</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="494" spans="1:4" x14ac:dyDescent="0.3">
@@ -13938,13 +13938,13 @@
         <v>1468</v>
       </c>
       <c r="B494" s="3" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="C494" s="2" t="s">
-        <v>2041</v>
+        <v>2038</v>
       </c>
       <c r="D494" s="2" t="s">
-        <v>2042</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="495" spans="1:4" x14ac:dyDescent="0.3">
@@ -13955,10 +13955,10 @@
         <v>1558</v>
       </c>
       <c r="C495" s="2" t="s">
-        <v>2043</v>
+        <v>2040</v>
       </c>
       <c r="D495" s="2" t="s">
-        <v>2044</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="496" spans="1:4" x14ac:dyDescent="0.3">
@@ -13966,13 +13966,13 @@
         <v>1517</v>
       </c>
       <c r="B496" s="3" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="C496" s="2" t="s">
-        <v>2045</v>
+        <v>2042</v>
       </c>
       <c r="D496" s="2" t="s">
-        <v>2046</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="497" spans="1:4" x14ac:dyDescent="0.3">
@@ -13980,13 +13980,13 @@
         <v>1536</v>
       </c>
       <c r="B497" s="3" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="C497" s="2" t="s">
-        <v>2047</v>
+        <v>2044</v>
       </c>
       <c r="D497" s="2" t="s">
-        <v>2048</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="498" spans="1:4" x14ac:dyDescent="0.3">
@@ -13994,13 +13994,13 @@
         <v>1442</v>
       </c>
       <c r="B498" s="3" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="C498" s="2" t="s">
-        <v>2049</v>
+        <v>2046</v>
       </c>
       <c r="D498" s="2" t="s">
-        <v>2050</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="499" spans="1:4" x14ac:dyDescent="0.3">
@@ -14008,13 +14008,13 @@
         <v>1432</v>
       </c>
       <c r="B499" s="3" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="C499" s="2" t="s">
-        <v>2051</v>
+        <v>2048</v>
       </c>
       <c r="D499" s="2" t="s">
-        <v>2052</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="500" spans="1:4" x14ac:dyDescent="0.3">
@@ -14022,13 +14022,13 @@
         <v>1368</v>
       </c>
       <c r="B500" s="3" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="C500" s="2" t="s">
-        <v>2053</v>
+        <v>2050</v>
       </c>
       <c r="D500" s="2" t="s">
-        <v>2054</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="501" spans="1:4" x14ac:dyDescent="0.3">
@@ -14036,13 +14036,13 @@
         <v>1394</v>
       </c>
       <c r="B501" s="3" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="C501" s="2" t="s">
-        <v>2055</v>
+        <v>2052</v>
       </c>
       <c r="D501" s="2" t="s">
-        <v>2056</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="502" spans="1:4" x14ac:dyDescent="0.3">
@@ -14050,13 +14050,13 @@
         <v>1439</v>
       </c>
       <c r="B502" s="3" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="C502" s="2" t="s">
-        <v>2057</v>
+        <v>2054</v>
       </c>
       <c r="D502" s="2" t="s">
-        <v>2058</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="503" spans="1:4" x14ac:dyDescent="0.3">
@@ -14064,13 +14064,13 @@
         <v>1499</v>
       </c>
       <c r="B503" s="3" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="C503" s="2" t="s">
-        <v>2059</v>
+        <v>2056</v>
       </c>
       <c r="D503" s="2" t="s">
-        <v>2060</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="504" spans="1:4" x14ac:dyDescent="0.3">
@@ -14081,10 +14081,10 @@
         <v>1546</v>
       </c>
       <c r="C504" s="2" t="s">
-        <v>2061</v>
+        <v>2058</v>
       </c>
       <c r="D504" s="2" t="s">
-        <v>2062</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="505" spans="1:4" x14ac:dyDescent="0.3">
@@ -14092,13 +14092,13 @@
         <v>1429</v>
       </c>
       <c r="B505" s="3" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="C505" s="2" t="s">
-        <v>2063</v>
+        <v>2060</v>
       </c>
       <c r="D505" s="2" t="s">
-        <v>2064</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="506" spans="1:4" x14ac:dyDescent="0.3">
@@ -14106,13 +14106,13 @@
         <v>1449</v>
       </c>
       <c r="B506" s="3" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="C506" s="2" t="s">
-        <v>2065</v>
+        <v>2062</v>
       </c>
       <c r="D506" s="2" t="s">
-        <v>2066</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="507" spans="1:4" x14ac:dyDescent="0.3">
@@ -14120,13 +14120,13 @@
         <v>1354</v>
       </c>
       <c r="B507" s="3" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="C507" s="2" t="s">
-        <v>2067</v>
+        <v>2064</v>
       </c>
       <c r="D507" s="2" t="s">
-        <v>2068</v>
+        <v>2065</v>
       </c>
     </row>
     <row r="508" spans="1:4" x14ac:dyDescent="0.3">
@@ -14137,10 +14137,10 @@
         <v>1553</v>
       </c>
       <c r="C508" s="2" t="s">
-        <v>2069</v>
+        <v>2066</v>
       </c>
       <c r="D508" s="2" t="s">
-        <v>2070</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="509" spans="1:4" x14ac:dyDescent="0.3">
@@ -14148,13 +14148,13 @@
         <v>1360</v>
       </c>
       <c r="B509" s="3" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="C509" s="2" t="s">
-        <v>2071</v>
+        <v>2068</v>
       </c>
       <c r="D509" s="2" t="s">
-        <v>2072</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="510" spans="1:4" x14ac:dyDescent="0.3">
@@ -14162,13 +14162,13 @@
         <v>1506</v>
       </c>
       <c r="B510" s="3" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="C510" s="2" t="s">
-        <v>2073</v>
+        <v>2070</v>
       </c>
       <c r="D510" s="2" t="s">
-        <v>2074</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="511" spans="1:4" x14ac:dyDescent="0.3">
@@ -14179,10 +14179,10 @@
         <v>1548</v>
       </c>
       <c r="C511" s="2" t="s">
-        <v>2075</v>
+        <v>2072</v>
       </c>
       <c r="D511" s="2" t="s">
-        <v>2076</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="512" spans="1:4" x14ac:dyDescent="0.3">
@@ -14190,13 +14190,13 @@
         <v>1427</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="C512" s="2" t="s">
-        <v>2077</v>
+        <v>2074</v>
       </c>
       <c r="D512" s="2" t="s">
-        <v>2078</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="513" spans="1:4" x14ac:dyDescent="0.3">
@@ -14204,13 +14204,13 @@
         <v>1486</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="C513" s="2" t="s">
-        <v>2079</v>
+        <v>2076</v>
       </c>
       <c r="D513" s="2" t="s">
-        <v>2080</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="514" spans="1:4" x14ac:dyDescent="0.3">
@@ -14218,13 +14218,13 @@
         <v>1374</v>
       </c>
       <c r="B514" s="3" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="C514" s="2" t="s">
-        <v>2081</v>
+        <v>2078</v>
       </c>
       <c r="D514" s="2" t="s">
-        <v>2082</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="515" spans="1:4" x14ac:dyDescent="0.3">
@@ -14232,13 +14232,13 @@
         <v>1436</v>
       </c>
       <c r="B515" s="3" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="C515" s="2" t="s">
-        <v>2083</v>
+        <v>2080</v>
       </c>
       <c r="D515" s="2" t="s">
-        <v>2084</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="516" spans="1:4" x14ac:dyDescent="0.3">
@@ -14246,13 +14246,13 @@
         <v>1420</v>
       </c>
       <c r="B516" s="3" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="C516" s="2" t="s">
-        <v>2085</v>
+        <v>2082</v>
       </c>
       <c r="D516" s="2" t="s">
-        <v>2086</v>
+        <v>2083</v>
       </c>
     </row>
     <row r="517" spans="1:4" x14ac:dyDescent="0.3">
@@ -14260,13 +14260,13 @@
         <v>1378</v>
       </c>
       <c r="B517" s="3" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="C517" s="2" t="s">
-        <v>2087</v>
+        <v>2084</v>
       </c>
       <c r="D517" s="2" t="s">
-        <v>2088</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="518" spans="1:4" x14ac:dyDescent="0.3">
@@ -14274,13 +14274,13 @@
         <v>1402</v>
       </c>
       <c r="B518" s="3" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="C518" s="2" t="s">
-        <v>2089</v>
+        <v>2086</v>
       </c>
       <c r="D518" s="2" t="s">
-        <v>2090</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="519" spans="1:4" x14ac:dyDescent="0.3">
@@ -14288,13 +14288,13 @@
         <v>1379</v>
       </c>
       <c r="B519" s="3" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="C519" s="2" t="s">
-        <v>2091</v>
+        <v>2088</v>
       </c>
       <c r="D519" s="2" t="s">
-        <v>2092</v>
+        <v>2089</v>
       </c>
     </row>
     <row r="520" spans="1:4" x14ac:dyDescent="0.3">
@@ -14302,13 +14302,13 @@
         <v>1357</v>
       </c>
       <c r="B520" s="3" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="C520" s="2" t="s">
-        <v>2093</v>
+        <v>2090</v>
       </c>
       <c r="D520" s="2" t="s">
-        <v>2094</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="521" spans="1:4" x14ac:dyDescent="0.3">
@@ -14316,13 +14316,13 @@
         <v>1370</v>
       </c>
       <c r="B521" s="3" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="C521" s="2" t="s">
-        <v>2095</v>
+        <v>2092</v>
       </c>
       <c r="D521" s="2" t="s">
-        <v>2096</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="522" spans="1:4" x14ac:dyDescent="0.3">
@@ -14330,13 +14330,13 @@
         <v>1444</v>
       </c>
       <c r="B522" s="3" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="C522" s="2" t="s">
-        <v>2097</v>
+        <v>2094</v>
       </c>
       <c r="D522" s="2" t="s">
-        <v>2098</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="523" spans="1:4" x14ac:dyDescent="0.3">
@@ -14344,13 +14344,13 @@
         <v>1408</v>
       </c>
       <c r="B523" s="3" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="C523" s="2" t="s">
-        <v>2099</v>
+        <v>2096</v>
       </c>
       <c r="D523" s="2" t="s">
-        <v>2100</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="524" spans="1:4" x14ac:dyDescent="0.3">
@@ -14358,13 +14358,13 @@
         <v>1389</v>
       </c>
       <c r="B524" s="3" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="C524" s="2" t="s">
-        <v>2101</v>
+        <v>2098</v>
       </c>
       <c r="D524" s="2" t="s">
-        <v>2102</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="525" spans="1:4" x14ac:dyDescent="0.3">
@@ -14372,13 +14372,13 @@
         <v>1369</v>
       </c>
       <c r="B525" s="3" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="C525" s="2" t="s">
-        <v>2103</v>
+        <v>2100</v>
       </c>
       <c r="D525" s="2" t="s">
-        <v>2104</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="526" spans="1:4" x14ac:dyDescent="0.3">
@@ -14389,10 +14389,10 @@
         <v>1543</v>
       </c>
       <c r="C526" s="2" t="s">
-        <v>2105</v>
+        <v>2102</v>
       </c>
       <c r="D526" s="2" t="s">
-        <v>2106</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="527" spans="1:4" x14ac:dyDescent="0.3">
@@ -14400,13 +14400,13 @@
         <v>1418</v>
       </c>
       <c r="B527" s="3" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="C527" s="2" t="s">
-        <v>2107</v>
+        <v>2104</v>
       </c>
       <c r="D527" s="2" t="s">
-        <v>2108</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="528" spans="1:4" x14ac:dyDescent="0.3">
@@ -14414,13 +14414,13 @@
         <v>1454</v>
       </c>
       <c r="B528" s="3" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
       <c r="C528" s="2" t="s">
-        <v>2109</v>
+        <v>2106</v>
       </c>
       <c r="D528" s="2" t="s">
-        <v>2110</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="529" spans="1:4" x14ac:dyDescent="0.3">
@@ -14428,13 +14428,13 @@
         <v>1497</v>
       </c>
       <c r="B529" s="3" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="C529" s="2" t="s">
-        <v>2111</v>
+        <v>2108</v>
       </c>
       <c r="D529" s="2" t="s">
-        <v>2112</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="530" spans="1:4" x14ac:dyDescent="0.3">
@@ -14442,13 +14442,13 @@
         <v>1440</v>
       </c>
       <c r="B530" s="3" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="C530" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
       <c r="D530" s="2" t="s">
-        <v>2114</v>
+        <v>2111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>